<commit_message>
modificación de harmony con archivo de excel modificado
</commit_message>
<xml_diff>
--- a/Ejemplo de costos.xlsx
+++ b/Ejemplo de costos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\PrimeroM_2021A-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98E23EEA-A12C-4E79-9601-F92D399638BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455D69DC-0213-49F1-8398-C57AC1162B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13550" yWindow="-3160" windowWidth="19420" windowHeight="11020" xr2:uid="{D7E7092C-B678-4A92-9ADE-E9E8369119DE}"/>
+    <workbookView xWindow="16870" yWindow="-1710" windowWidth="15380" windowHeight="8330" xr2:uid="{D7E7092C-B678-4A92-9ADE-E9E8369119DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Costos fijos</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Utilidad total</t>
+  </si>
+  <si>
+    <t>Ejemplo de cosotos unitarios</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0C4FC7-2823-4287-8363-420784DF3F10}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,47 +529,50 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="1">
         <v>1200000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>400000</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -581,7 +587,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -597,7 +603,7 @@
         <v>56.666666666666664</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -606,7 +612,7 @@
         <v>470588.23529411765</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>9</v>
       </c>
@@ -615,7 +621,7 @@
         <v>143.33333333333334</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>10</v>
       </c>

</xml_diff>